<commit_message>
starting work on MA / Simple exponential smoothing
</commit_message>
<xml_diff>
--- a/src/generated_spreadsheet.xlsx
+++ b/src/generated_spreadsheet.xlsx
@@ -758,6 +758,9 @@
       <c r="B5">
         <v>34000</v>
       </c>
+      <c r="C5">
+        <v>19500</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
@@ -766,6 +769,15 @@
       <c r="B6">
         <v>10000</v>
       </c>
+      <c r="C6">
+        <v>20000</v>
+      </c>
+      <c r="D6">
+        <v>9500</v>
+      </c>
+      <c r="E6">
+        <v>9500</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
@@ -774,6 +786,15 @@
       <c r="B7">
         <v>18000</v>
       </c>
+      <c r="C7">
+        <v>21250</v>
+      </c>
+      <c r="D7">
+        <v>2000</v>
+      </c>
+      <c r="E7">
+        <v>2000</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
@@ -782,6 +803,15 @@
       <c r="B8">
         <v>23000</v>
       </c>
+      <c r="C8">
+        <v>21250</v>
+      </c>
+      <c r="D8">
+        <v>-1750</v>
+      </c>
+      <c r="E8">
+        <v>1750</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9">
@@ -790,6 +820,15 @@
       <c r="B9">
         <v>38000</v>
       </c>
+      <c r="C9">
+        <v>22250</v>
+      </c>
+      <c r="D9">
+        <v>-16750</v>
+      </c>
+      <c r="E9">
+        <v>16750</v>
+      </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
@@ -798,6 +837,15 @@
       <c r="B10">
         <v>12000</v>
       </c>
+      <c r="C10">
+        <v>22750</v>
+      </c>
+      <c r="D10">
+        <v>10250</v>
+      </c>
+      <c r="E10">
+        <v>10250</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
@@ -806,6 +854,15 @@
       <c r="B11">
         <v>13000</v>
       </c>
+      <c r="C11">
+        <v>21500</v>
+      </c>
+      <c r="D11">
+        <v>9750</v>
+      </c>
+      <c r="E11">
+        <v>9750</v>
+      </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12">
@@ -814,6 +871,15 @@
       <c r="B12">
         <v>32000</v>
       </c>
+      <c r="C12">
+        <v>23750</v>
+      </c>
+      <c r="D12">
+        <v>-10500</v>
+      </c>
+      <c r="E12">
+        <v>10500</v>
+      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13">
@@ -821,6 +887,15 @@
       </c>
       <c r="B13">
         <v>41000</v>
+      </c>
+      <c r="C13">
+        <v>24500</v>
+      </c>
+      <c r="D13">
+        <v>-17250</v>
+      </c>
+      <c r="E13">
+        <v>17250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost done with ma
</commit_message>
<xml_diff>
--- a/src/generated_spreadsheet.xlsx
+++ b/src/generated_spreadsheet.xlsx
@@ -773,13 +773,22 @@
         <v>20000</v>
       </c>
       <c r="D6">
-        <v>9500</v>
+        <v>19500</v>
       </c>
       <c r="E6">
         <v>9500</v>
       </c>
       <c r="F6">
+        <v>9500</v>
+      </c>
+      <c r="G6">
         <v>90250000</v>
+      </c>
+      <c r="H6">
+        <v>9500</v>
+      </c>
+      <c r="I6">
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -793,13 +802,22 @@
         <v>21250</v>
       </c>
       <c r="D7">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="E7">
         <v>2000</v>
       </c>
       <c r="F7">
+        <v>2000</v>
+      </c>
+      <c r="G7">
         <v>47125000</v>
+      </c>
+      <c r="H7">
+        <v>5750</v>
+      </c>
+      <c r="I7">
+        <v>11.11111111111111</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -813,13 +831,22 @@
         <v>21250</v>
       </c>
       <c r="D8">
+        <v>21250</v>
+      </c>
+      <c r="E8">
         <v>-1750</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>1750</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>32437500</v>
+      </c>
+      <c r="H8">
+        <v>4416.666666666667</v>
+      </c>
+      <c r="I8">
+        <v>7.608695652173914</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -833,13 +860,22 @@
         <v>22250</v>
       </c>
       <c r="D9">
+        <v>21250</v>
+      </c>
+      <c r="E9">
         <v>-16750</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>16750</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>94468750</v>
+      </c>
+      <c r="H9">
+        <v>7500</v>
+      </c>
+      <c r="I9">
+        <v>44.07894736842105</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -853,13 +889,22 @@
         <v>22750</v>
       </c>
       <c r="D10">
-        <v>10250</v>
+        <v>22250</v>
       </c>
       <c r="E10">
         <v>10250</v>
       </c>
       <c r="F10">
+        <v>10250</v>
+      </c>
+      <c r="G10">
         <v>96587500</v>
+      </c>
+      <c r="H10">
+        <v>8050</v>
+      </c>
+      <c r="I10">
+        <v>85.41666666666666</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -873,13 +918,22 @@
         <v>21500</v>
       </c>
       <c r="D11">
-        <v>9750</v>
+        <v>22750</v>
       </c>
       <c r="E11">
         <v>9750</v>
       </c>
       <c r="F11">
+        <v>9750</v>
+      </c>
+      <c r="G11">
         <v>96333333.33333333</v>
+      </c>
+      <c r="H11">
+        <v>8333.333333333334</v>
+      </c>
+      <c r="I11">
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -893,13 +947,22 @@
         <v>23750</v>
       </c>
       <c r="D12">
+        <v>21500</v>
+      </c>
+      <c r="E12">
         <v>-10500</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>10500</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>98321428.57142857</v>
+      </c>
+      <c r="H12">
+        <v>8642.857142857143</v>
+      </c>
+      <c r="I12">
+        <v>32.8125</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -913,13 +976,22 @@
         <v>24500</v>
       </c>
       <c r="D13">
+        <v>23750</v>
+      </c>
+      <c r="E13">
         <v>-17250</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>17250</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>123226562.5</v>
+      </c>
+      <c r="H13">
+        <v>9718.75</v>
+      </c>
+      <c r="I13">
+        <v>42.07317073170731</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
instead of showing figures through tk, generate pictures and export them
</commit_message>
<xml_diff>
--- a/src/generated_spreadsheet.xlsx
+++ b/src/generated_spreadsheet.xlsx
@@ -1095,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>22083</v>
+        <v>22083.33333333333</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1106,28 +1106,28 @@
         <v>8000</v>
       </c>
       <c r="C3">
-        <v>20674.7</v>
+        <v>20675</v>
       </c>
       <c r="D3">
-        <v>22083</v>
+        <v>22083.33333333333</v>
       </c>
       <c r="E3">
-        <v>14083</v>
+        <v>14083.33333333333</v>
       </c>
       <c r="F3">
-        <v>14083</v>
+        <v>14083.33333333333</v>
       </c>
       <c r="G3">
-        <v>198330889</v>
+        <v>198340277.7777777</v>
       </c>
       <c r="H3">
-        <v>14083</v>
+        <v>14083.33333333333</v>
       </c>
       <c r="I3">
-        <v>176.0375</v>
+        <v>176.0416666666667</v>
       </c>
       <c r="J3">
-        <v>176.0375</v>
+        <v>176.0416666666667</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -1141,28 +1141,28 @@
         <v>13000</v>
       </c>
       <c r="C4">
-        <v>19907.23</v>
+        <v>19907.5</v>
       </c>
       <c r="D4">
-        <v>20674.7</v>
+        <v>20675</v>
       </c>
       <c r="E4">
-        <v>7674.700000000001</v>
+        <v>7675</v>
       </c>
       <c r="F4">
-        <v>7674.700000000001</v>
+        <v>7675</v>
       </c>
       <c r="G4">
-        <v>128615954.545</v>
+        <v>128622951.3888889</v>
       </c>
       <c r="H4">
-        <v>10878.85</v>
+        <v>10879.16666666667</v>
       </c>
       <c r="I4">
-        <v>59.03615384615385</v>
+        <v>59.03846153846154</v>
       </c>
       <c r="J4">
-        <v>117.5368269230769</v>
+        <v>117.5400641025641</v>
       </c>
       <c r="K4">
         <v>2</v>
@@ -1176,31 +1176,31 @@
         <v>23000</v>
       </c>
       <c r="C5">
-        <v>20216.507</v>
+        <v>20216.75</v>
       </c>
       <c r="D5">
-        <v>19907.23</v>
+        <v>19907.5</v>
       </c>
       <c r="E5">
-        <v>-3092.77</v>
+        <v>-3092.5</v>
       </c>
       <c r="F5">
-        <v>3092.77</v>
+        <v>3092.5</v>
       </c>
       <c r="G5">
-        <v>88932378.4543</v>
+        <v>88936486.34259258</v>
       </c>
       <c r="H5">
-        <v>8283.49</v>
+        <v>8283.611111111111</v>
       </c>
       <c r="I5">
-        <v>13.44682608695652</v>
+        <v>13.44565217391304</v>
       </c>
       <c r="J5">
-        <v>82.84015997770345</v>
+        <v>82.84192679301374</v>
       </c>
       <c r="K5">
-        <v>2.253268851655522</v>
+        <v>2.253344958250897</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1211,31 +1211,31 @@
         <v>34000</v>
       </c>
       <c r="C6">
-        <v>21594.8563</v>
+        <v>21595.075</v>
       </c>
       <c r="D6">
-        <v>20216.507</v>
+        <v>20216.75</v>
       </c>
       <c r="E6">
-        <v>-13783.493</v>
+        <v>-13783.25</v>
       </c>
       <c r="F6">
-        <v>13783.493</v>
+        <v>13783.25</v>
       </c>
       <c r="G6">
-        <v>114195453.6609872</v>
+        <v>114196859.8975694</v>
       </c>
       <c r="H6">
-        <v>9658.490750000001</v>
+        <v>9658.520833333332</v>
       </c>
       <c r="I6">
-        <v>40.53968529411765</v>
+        <v>40.53897058823529</v>
       </c>
       <c r="J6">
-        <v>72.26504130680701</v>
+        <v>72.26618774181914</v>
       </c>
       <c r="K6">
-        <v>0.5054037039896737</v>
+        <v>0.5055208160324756</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1246,31 +1246,31 @@
         <v>10000</v>
       </c>
       <c r="C7">
-        <v>20435.37067</v>
+        <v>20435.5675</v>
       </c>
       <c r="D7">
-        <v>21594.8563</v>
+        <v>21595.075</v>
       </c>
       <c r="E7">
-        <v>11594.8563</v>
+        <v>11595.075</v>
       </c>
       <c r="F7">
-        <v>11594.8563</v>
+        <v>11595.075</v>
       </c>
       <c r="G7">
-        <v>118244501.4523197</v>
+        <v>118246640.7691805</v>
       </c>
       <c r="H7">
-        <v>10045.76386</v>
+        <v>10045.83166666667</v>
       </c>
       <c r="I7">
-        <v>115.948563</v>
+        <v>115.95075</v>
       </c>
       <c r="J7">
-        <v>81.00174564544561</v>
+        <v>81.00310019345531</v>
       </c>
       <c r="K7">
-        <v>1.640123491813793</v>
+        <v>1.640248301990594</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1281,31 +1281,31 @@
         <v>18000</v>
       </c>
       <c r="C8">
-        <v>20191.833603</v>
+        <v>20192.01075</v>
       </c>
       <c r="D8">
-        <v>20435.37067</v>
+        <v>20435.5675</v>
       </c>
       <c r="E8">
-        <v>2435.370670000004</v>
+        <v>2435.567500000001</v>
       </c>
       <c r="F8">
-        <v>2435.370670000004</v>
+        <v>2435.567500000001</v>
       </c>
       <c r="G8">
-        <v>99525589.59364916</v>
+        <v>99527532.14882648</v>
       </c>
       <c r="H8">
-        <v>8777.364995000002</v>
+        <v>8777.454305555555</v>
       </c>
       <c r="I8">
-        <v>13.52983705555558</v>
+        <v>13.53093055555556</v>
       </c>
       <c r="J8">
-        <v>69.7564275471306</v>
+        <v>69.75773858713869</v>
       </c>
       <c r="K8">
-        <v>2.154594685395102</v>
+        <v>2.154750702759284</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1316,31 +1316,31 @@
         <v>23000</v>
       </c>
       <c r="C9">
-        <v>20472.6502427</v>
+        <v>20472.809675</v>
       </c>
       <c r="D9">
-        <v>20191.833603</v>
+        <v>20192.01075</v>
       </c>
       <c r="E9">
-        <v>-2808.166396999997</v>
+        <v>-2807.989249999999</v>
       </c>
       <c r="F9">
-        <v>2808.166396999997</v>
+        <v>2807.989249999999</v>
       </c>
       <c r="G9">
-        <v>86434190.86787643</v>
+        <v>86435713.78872491</v>
       </c>
       <c r="H9">
-        <v>7924.622338142857</v>
+        <v>7924.673583333332</v>
       </c>
       <c r="I9">
-        <v>12.20941911739129</v>
+        <v>12.20864891304347</v>
       </c>
       <c r="J9">
-        <v>61.53542634288213</v>
+        <v>61.53644006226795</v>
       </c>
       <c r="K9">
-        <v>2.032083913386071</v>
+        <v>2.032290215360395</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1351,31 +1351,31 @@
         <v>38000</v>
       </c>
       <c r="C10">
-        <v>22225.38521843</v>
+        <v>22225.5287075</v>
       </c>
       <c r="D10">
-        <v>20472.6502427</v>
+        <v>20472.809675</v>
       </c>
       <c r="E10">
-        <v>-17527.3497573</v>
+        <v>-17527.190325</v>
       </c>
       <c r="F10">
-        <v>17527.3497573</v>
+        <v>17527.190325</v>
       </c>
       <c r="G10">
-        <v>114030915.6987324</v>
+        <v>114031549.651231</v>
       </c>
       <c r="H10">
-        <v>9124.963265537501</v>
+        <v>9124.988176041667</v>
       </c>
       <c r="I10">
-        <v>46.12460462447368</v>
+        <v>46.12418506578948</v>
       </c>
       <c r="J10">
-        <v>59.60907362808108</v>
+        <v>59.60990818770814</v>
       </c>
       <c r="K10">
-        <v>-0.1560392237059725</v>
+        <v>-0.1558307489537476</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1386,31 +1386,31 @@
         <v>12000</v>
       </c>
       <c r="C11">
-        <v>21202.846696587</v>
+        <v>21202.97583675</v>
       </c>
       <c r="D11">
-        <v>22225.38521843</v>
+        <v>22225.5287075</v>
       </c>
       <c r="E11">
-        <v>10225.38521843</v>
+        <v>10225.5287075</v>
       </c>
       <c r="F11">
-        <v>10225.38521843</v>
+        <v>10225.5287075</v>
       </c>
       <c r="G11">
-        <v>112978425.3839051</v>
+        <v>112979314.9508616</v>
       </c>
       <c r="H11">
-        <v>9247.232371414446</v>
+        <v>9247.270457314815</v>
       </c>
       <c r="I11">
-        <v>85.21154348691667</v>
+        <v>85.21273922916667</v>
       </c>
       <c r="J11">
-        <v>62.45379250128503</v>
+        <v>62.45466719231464</v>
       </c>
       <c r="K11">
-        <v>0.9518018668307501</v>
+        <v>0.9520187612626271</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1421,31 +1421,31 @@
         <v>13000</v>
       </c>
       <c r="C12">
-        <v>20382.5620269283</v>
+        <v>20382.678253075</v>
       </c>
       <c r="D12">
-        <v>21202.846696587</v>
+        <v>21202.97583675</v>
       </c>
       <c r="E12">
-        <v>8202.846696587003</v>
+        <v>8202.975836750004</v>
       </c>
       <c r="F12">
-        <v>8202.846696587003</v>
+        <v>8202.975836750004</v>
       </c>
       <c r="G12">
-        <v>108409252.2382855</v>
+        <v>108410264.7136059</v>
       </c>
       <c r="H12">
-        <v>9142.793803931701</v>
+        <v>9142.840995258335</v>
       </c>
       <c r="I12">
-        <v>63.09882074297695</v>
+        <v>63.09981412884618</v>
       </c>
       <c r="J12">
-        <v>62.51829532545422</v>
+        <v>62.5191818859678</v>
       </c>
       <c r="K12">
-        <v>1.859866917637864</v>
+        <v>1.860094779227079</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1456,31 +1456,31 @@
         <v>32000</v>
       </c>
       <c r="C13">
-        <v>21544.30582423547</v>
+        <v>21544.4104277675</v>
       </c>
       <c r="D13">
-        <v>20382.5620269283</v>
+        <v>20382.678253075</v>
       </c>
       <c r="E13">
-        <v>-11617.4379730717</v>
+        <v>-11617.321746925</v>
       </c>
       <c r="F13">
-        <v>11617.4379730717</v>
+        <v>11617.321746925</v>
       </c>
       <c r="G13">
-        <v>110823398.8582748</v>
+        <v>110824073.7916033</v>
       </c>
       <c r="H13">
-        <v>9367.7614556717</v>
+        <v>9367.793790864394</v>
       </c>
       <c r="I13">
-        <v>36.30449366584905</v>
+        <v>36.30413045914062</v>
       </c>
       <c r="J13">
-        <v>60.13522244730829</v>
+        <v>60.13599539261987</v>
       </c>
       <c r="K13">
-        <v>0.575051124341323</v>
+        <v>0.5752933055501281</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1491,31 +1491,31 @@
         <v>41000</v>
       </c>
       <c r="C14">
-        <v>23489.87524181193</v>
+        <v>23489.96938499075</v>
       </c>
       <c r="D14">
-        <v>21544.30582423547</v>
+        <v>21544.4104277675</v>
       </c>
       <c r="E14">
-        <v>-19455.69417576453</v>
+        <v>-19455.5895722325</v>
       </c>
       <c r="F14">
-        <v>19455.69417576453</v>
+        <v>19455.5895722325</v>
       </c>
       <c r="G14">
-        <v>133131785.2751584</v>
+        <v>133132064.7758998</v>
       </c>
       <c r="H14">
-        <v>10208.42251567944</v>
+        <v>10208.44343931174</v>
       </c>
       <c r="I14">
-        <v>47.45291262381592</v>
+        <v>47.45265749324999</v>
       </c>
       <c r="J14">
-        <v>59.07836329535059</v>
+        <v>59.07905056767238</v>
       </c>
       <c r="K14">
-        <v>-1.378151462335201</v>
+        <v>-1.377914331425489</v>
       </c>
     </row>
   </sheetData>

</xml_diff>